<commit_message>
maris db global dump handler
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_detection.xlsx
+++ b/nbs/files/lut/dbo_detection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5B654-27B9-4147-A8EB-379D0EAB74EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD9F567-C948-EA48-B649-7F03986DEB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="dbo_detection" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dbo_biogroup">dbo_detection!$A$1:$B$5</definedName>
+    <definedName name="dbo_biogroup">dbo_detection!$A$1:$B$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>detection_id</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Not detected and no reading</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Not available</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,13 +487,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -495,10 +498,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -506,10 +512,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -517,9 +523,20 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -529,21 +546,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="627c5da731661f4bf76604184727f2d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf665a11c7ceb3b31f5a9dbdfc3fcda" ns2:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -675,24 +677,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B23956F3-18E7-4AFD-ADCE-F3B49C2803C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9BC7497-056F-4771-800C-81EB0B6B6871}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1440613E-EE35-442E-92C2-BEA114BE45FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -708,4 +708,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9BC7497-056F-4771-800C-81EB0B6B6871}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B23956F3-18E7-4AFD-ADCE-F3B49C2803C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>